<commit_message>
feat(condo): DOMA-4452 added meter place for import
</commit_message>
<xml_diff>
--- a/apps/condo/public/meter-import-example-en.xlsx
+++ b/apps/condo/public/meter-import-example-en.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
   <si>
     <t>Address</t>
   </si>
@@ -67,6 +67,9 @@
     <t>Control readings date</t>
   </si>
   <si>
+    <t>Meter place</t>
+  </si>
+  <si>
     <t>г Москва, ул Тверская, д 1</t>
   </si>
   <si>
@@ -92,6 +95,12 @@
   </si>
   <si>
     <t>2021-01-25</t>
+  </si>
+  <si>
+    <t>Kitchen</t>
+  </si>
+  <si>
+    <t>Bathroom</t>
   </si>
   <si>
     <t>CW</t>
@@ -142,9 +151,9 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="15"/>
+      <sz val="13"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="10"/>
@@ -543,6 +552,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -572,6 +582,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -597,6 +608,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -622,6 +634,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -647,6 +660,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -672,6 +686,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -697,6 +712,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -722,6 +738,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -747,6 +764,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -772,6 +790,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -822,6 +841,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -847,6 +867,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -872,6 +893,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -897,6 +919,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -922,6 +945,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -947,6 +971,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -972,6 +997,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -997,6 +1023,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1022,6 +1049,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1047,6 +1075,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1094,6 +1123,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1123,6 +1153,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1148,6 +1179,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1173,6 +1205,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1198,6 +1231,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1223,6 +1257,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1248,6 +1283,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1273,6 +1309,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1298,6 +1335,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1323,6 +1361,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1351,7 +1390,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1371,8 +1410,8 @@
     <col min="15" max="15" width="12.8516" style="1" customWidth="1"/>
     <col min="16" max="16" width="22.1719" style="1" customWidth="1"/>
     <col min="17" max="17" width="18.1719" style="1" customWidth="1"/>
-    <col min="18" max="18" width="23.5" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="14.5" style="1" customWidth="1"/>
+    <col min="18" max="19" width="23.5" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.75" customHeight="1">
@@ -1430,22 +1469,25 @@
       <c r="R1" t="s" s="7">
         <v>17</v>
       </c>
+      <c r="S1" t="s" s="7">
+        <v>18</v>
+      </c>
     </row>
     <row r="2" ht="13.75" customHeight="1">
       <c r="A2" t="s" s="8">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
       </c>
       <c r="C2" t="s" s="8">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" s="9">
         <v>111</v>
       </c>
       <c r="E2" t="s" s="8">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" s="9">
         <v>1</v>
@@ -1460,42 +1502,45 @@
       <c r="J2" s="11"/>
       <c r="K2" s="11"/>
       <c r="L2" t="s" s="7">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M2" s="12">
         <v>44216</v>
       </c>
       <c r="N2" t="s" s="7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O2" t="s" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P2" t="s" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q2" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R2" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="S2" t="s" s="7">
+        <v>28</v>
       </c>
     </row>
     <row r="3" ht="13.75" customHeight="1">
       <c r="A3" t="s" s="7">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="10">
         <v>1</v>
       </c>
       <c r="C3" t="s" s="7">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" s="10">
         <v>111</v>
       </c>
       <c r="E3" t="s" s="7">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F3" s="10">
         <v>1</v>
@@ -1510,42 +1555,45 @@
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
       <c r="L3" t="s" s="7">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M3" s="12">
         <v>44216</v>
       </c>
       <c r="N3" t="s" s="7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O3" t="s" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P3" t="s" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q3" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R3" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="S3" t="s" s="7">
+        <v>29</v>
       </c>
     </row>
     <row r="4" ht="13.75" customHeight="1">
       <c r="A4" t="s" s="7">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="10">
         <v>1</v>
       </c>
       <c r="C4" t="s" s="7">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" s="10">
         <v>111</v>
       </c>
       <c r="E4" t="s" s="7">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F4" s="10">
         <v>2</v>
@@ -1560,42 +1608,45 @@
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
       <c r="L4" t="s" s="7">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M4" s="12">
         <v>44216</v>
       </c>
       <c r="N4" t="s" s="7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O4" t="s" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P4" t="s" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q4" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R4" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="S4" t="s" s="7">
+        <v>28</v>
       </c>
     </row>
     <row r="5" ht="13.75" customHeight="1">
       <c r="A5" t="s" s="7">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="10">
         <v>1</v>
       </c>
       <c r="C5" t="s" s="7">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" s="10">
         <v>111</v>
       </c>
       <c r="E5" t="s" s="7">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F5" s="10">
         <v>2</v>
@@ -1610,42 +1661,45 @@
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
       <c r="L5" t="s" s="7">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M5" s="12">
         <v>44216</v>
       </c>
       <c r="N5" t="s" s="7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O5" t="s" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P5" t="s" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q5" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R5" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="S5" t="s" s="7">
+        <v>29</v>
       </c>
     </row>
     <row r="6" ht="13.75" customHeight="1">
       <c r="A6" t="s" s="7">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="10">
         <v>1</v>
       </c>
       <c r="C6" t="s" s="7">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" s="10">
         <v>111</v>
       </c>
       <c r="E6" t="s" s="7">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F6" s="10">
         <v>2</v>
@@ -1664,42 +1718,45 @@
       </c>
       <c r="K6" s="11"/>
       <c r="L6" t="s" s="7">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="M6" s="12">
         <v>44216</v>
       </c>
       <c r="N6" t="s" s="7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O6" t="s" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P6" t="s" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q6" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R6" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="S6" t="s" s="7">
+        <v>28</v>
       </c>
     </row>
     <row r="7" ht="13.75" customHeight="1">
       <c r="A7" t="s" s="7">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="10">
         <v>1</v>
       </c>
       <c r="C7" t="s" s="7">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" s="10">
         <v>111</v>
       </c>
       <c r="E7" t="s" s="7">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F7" s="10">
         <v>2</v>
@@ -1724,36 +1781,39 @@
         <v>44216</v>
       </c>
       <c r="N7" t="s" s="7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O7" t="s" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P7" t="s" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q7" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R7" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="S7" t="s" s="7">
+        <v>29</v>
       </c>
     </row>
     <row r="8" ht="13.75" customHeight="1">
       <c r="A8" t="s" s="7">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B8" s="10">
         <v>2</v>
       </c>
       <c r="C8" t="s" s="7">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D8" s="10">
         <v>222</v>
       </c>
       <c r="E8" t="s" s="7">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F8" s="10">
         <v>11</v>
@@ -1772,42 +1832,45 @@
       </c>
       <c r="K8" s="11"/>
       <c r="L8" t="s" s="7">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="M8" s="12">
         <v>44216</v>
       </c>
       <c r="N8" t="s" s="7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O8" t="s" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P8" t="s" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q8" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R8" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="S8" t="s" s="7">
+        <v>28</v>
       </c>
     </row>
     <row r="9" ht="13.75" customHeight="1">
       <c r="A9" t="s" s="7">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B9" s="10">
         <v>2</v>
       </c>
       <c r="C9" t="s" s="7">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D9" s="10">
         <v>222</v>
       </c>
       <c r="E9" t="s" s="7">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F9" s="10">
         <v>11</v>
@@ -1822,42 +1885,45 @@
       <c r="J9" s="11"/>
       <c r="K9" s="11"/>
       <c r="L9" t="s" s="7">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="M9" s="12">
         <v>44216</v>
       </c>
       <c r="N9" t="s" s="7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O9" t="s" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P9" t="s" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q9" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R9" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="S9" t="s" s="7">
+        <v>29</v>
       </c>
     </row>
     <row r="10" ht="13.75" customHeight="1">
       <c r="A10" t="s" s="7">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B10" s="10">
         <v>2</v>
       </c>
       <c r="C10" t="s" s="7">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D10" s="10">
         <v>222</v>
       </c>
       <c r="E10" t="s" s="7">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F10" s="10">
         <v>22</v>
@@ -1872,42 +1938,45 @@
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
       <c r="L10" t="s" s="7">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M10" s="12">
         <v>44216</v>
       </c>
       <c r="N10" t="s" s="7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O10" t="s" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P10" t="s" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q10" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R10" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="S10" t="s" s="7">
+        <v>28</v>
       </c>
     </row>
     <row r="11" ht="13.75" customHeight="1">
       <c r="A11" t="s" s="7">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B11" s="10">
         <v>2</v>
       </c>
       <c r="C11" t="s" s="7">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D11" s="10">
         <v>222</v>
       </c>
       <c r="E11" t="s" s="7">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F11" s="10">
         <v>33</v>
@@ -1922,25 +1991,28 @@
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
       <c r="L11" t="s" s="7">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M11" s="12">
         <v>44216</v>
       </c>
       <c r="N11" t="s" s="7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O11" t="s" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P11" t="s" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q11" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R11" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="S11" t="s" s="7">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(condo): DOMA-4452 added meter place for import (#3408)
</commit_message>
<xml_diff>
--- a/apps/condo/public/meter-import-example-en.xlsx
+++ b/apps/condo/public/meter-import-example-en.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
   <si>
     <t>Address</t>
   </si>
@@ -67,6 +67,9 @@
     <t>Control readings date</t>
   </si>
   <si>
+    <t>Meter place</t>
+  </si>
+  <si>
     <t>г Москва, ул Тверская, д 1</t>
   </si>
   <si>
@@ -92,6 +95,12 @@
   </si>
   <si>
     <t>2021-01-25</t>
+  </si>
+  <si>
+    <t>Kitchen</t>
+  </si>
+  <si>
+    <t>Bathroom</t>
   </si>
   <si>
     <t>CW</t>
@@ -142,9 +151,9 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="15"/>
+      <sz val="13"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="10"/>
@@ -543,6 +552,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -572,6 +582,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -597,6 +608,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -622,6 +634,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -647,6 +660,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -672,6 +686,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -697,6 +712,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -722,6 +738,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -747,6 +764,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -772,6 +790,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -822,6 +841,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -847,6 +867,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -872,6 +893,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -897,6 +919,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -922,6 +945,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -947,6 +971,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -972,6 +997,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -997,6 +1023,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1022,6 +1049,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1047,6 +1075,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1094,6 +1123,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1123,6 +1153,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1148,6 +1179,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1173,6 +1205,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1198,6 +1231,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1223,6 +1257,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1248,6 +1283,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1273,6 +1309,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1298,6 +1335,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1323,6 +1361,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1351,7 +1390,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1371,8 +1410,8 @@
     <col min="15" max="15" width="12.8516" style="1" customWidth="1"/>
     <col min="16" max="16" width="22.1719" style="1" customWidth="1"/>
     <col min="17" max="17" width="18.1719" style="1" customWidth="1"/>
-    <col min="18" max="18" width="23.5" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="14.5" style="1" customWidth="1"/>
+    <col min="18" max="19" width="23.5" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.75" customHeight="1">
@@ -1430,22 +1469,25 @@
       <c r="R1" t="s" s="7">
         <v>17</v>
       </c>
+      <c r="S1" t="s" s="7">
+        <v>18</v>
+      </c>
     </row>
     <row r="2" ht="13.75" customHeight="1">
       <c r="A2" t="s" s="8">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
       </c>
       <c r="C2" t="s" s="8">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" s="9">
         <v>111</v>
       </c>
       <c r="E2" t="s" s="8">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" s="9">
         <v>1</v>
@@ -1460,42 +1502,45 @@
       <c r="J2" s="11"/>
       <c r="K2" s="11"/>
       <c r="L2" t="s" s="7">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M2" s="12">
         <v>44216</v>
       </c>
       <c r="N2" t="s" s="7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O2" t="s" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P2" t="s" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q2" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R2" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="S2" t="s" s="7">
+        <v>28</v>
       </c>
     </row>
     <row r="3" ht="13.75" customHeight="1">
       <c r="A3" t="s" s="7">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="10">
         <v>1</v>
       </c>
       <c r="C3" t="s" s="7">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" s="10">
         <v>111</v>
       </c>
       <c r="E3" t="s" s="7">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F3" s="10">
         <v>1</v>
@@ -1510,42 +1555,45 @@
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
       <c r="L3" t="s" s="7">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M3" s="12">
         <v>44216</v>
       </c>
       <c r="N3" t="s" s="7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O3" t="s" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P3" t="s" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q3" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R3" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="S3" t="s" s="7">
+        <v>29</v>
       </c>
     </row>
     <row r="4" ht="13.75" customHeight="1">
       <c r="A4" t="s" s="7">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="10">
         <v>1</v>
       </c>
       <c r="C4" t="s" s="7">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" s="10">
         <v>111</v>
       </c>
       <c r="E4" t="s" s="7">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F4" s="10">
         <v>2</v>
@@ -1560,42 +1608,45 @@
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
       <c r="L4" t="s" s="7">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M4" s="12">
         <v>44216</v>
       </c>
       <c r="N4" t="s" s="7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O4" t="s" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P4" t="s" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q4" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R4" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="S4" t="s" s="7">
+        <v>28</v>
       </c>
     </row>
     <row r="5" ht="13.75" customHeight="1">
       <c r="A5" t="s" s="7">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="10">
         <v>1</v>
       </c>
       <c r="C5" t="s" s="7">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" s="10">
         <v>111</v>
       </c>
       <c r="E5" t="s" s="7">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F5" s="10">
         <v>2</v>
@@ -1610,42 +1661,45 @@
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
       <c r="L5" t="s" s="7">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M5" s="12">
         <v>44216</v>
       </c>
       <c r="N5" t="s" s="7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O5" t="s" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P5" t="s" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q5" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R5" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="S5" t="s" s="7">
+        <v>29</v>
       </c>
     </row>
     <row r="6" ht="13.75" customHeight="1">
       <c r="A6" t="s" s="7">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="10">
         <v>1</v>
       </c>
       <c r="C6" t="s" s="7">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" s="10">
         <v>111</v>
       </c>
       <c r="E6" t="s" s="7">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F6" s="10">
         <v>2</v>
@@ -1664,42 +1718,45 @@
       </c>
       <c r="K6" s="11"/>
       <c r="L6" t="s" s="7">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="M6" s="12">
         <v>44216</v>
       </c>
       <c r="N6" t="s" s="7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O6" t="s" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P6" t="s" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q6" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R6" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="S6" t="s" s="7">
+        <v>28</v>
       </c>
     </row>
     <row r="7" ht="13.75" customHeight="1">
       <c r="A7" t="s" s="7">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="10">
         <v>1</v>
       </c>
       <c r="C7" t="s" s="7">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" s="10">
         <v>111</v>
       </c>
       <c r="E7" t="s" s="7">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F7" s="10">
         <v>2</v>
@@ -1724,36 +1781,39 @@
         <v>44216</v>
       </c>
       <c r="N7" t="s" s="7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O7" t="s" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P7" t="s" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q7" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R7" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="S7" t="s" s="7">
+        <v>29</v>
       </c>
     </row>
     <row r="8" ht="13.75" customHeight="1">
       <c r="A8" t="s" s="7">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B8" s="10">
         <v>2</v>
       </c>
       <c r="C8" t="s" s="7">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D8" s="10">
         <v>222</v>
       </c>
       <c r="E8" t="s" s="7">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F8" s="10">
         <v>11</v>
@@ -1772,42 +1832,45 @@
       </c>
       <c r="K8" s="11"/>
       <c r="L8" t="s" s="7">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="M8" s="12">
         <v>44216</v>
       </c>
       <c r="N8" t="s" s="7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O8" t="s" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P8" t="s" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q8" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R8" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="S8" t="s" s="7">
+        <v>28</v>
       </c>
     </row>
     <row r="9" ht="13.75" customHeight="1">
       <c r="A9" t="s" s="7">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B9" s="10">
         <v>2</v>
       </c>
       <c r="C9" t="s" s="7">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D9" s="10">
         <v>222</v>
       </c>
       <c r="E9" t="s" s="7">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F9" s="10">
         <v>11</v>
@@ -1822,42 +1885,45 @@
       <c r="J9" s="11"/>
       <c r="K9" s="11"/>
       <c r="L9" t="s" s="7">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="M9" s="12">
         <v>44216</v>
       </c>
       <c r="N9" t="s" s="7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O9" t="s" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P9" t="s" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q9" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R9" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="S9" t="s" s="7">
+        <v>29</v>
       </c>
     </row>
     <row r="10" ht="13.75" customHeight="1">
       <c r="A10" t="s" s="7">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B10" s="10">
         <v>2</v>
       </c>
       <c r="C10" t="s" s="7">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D10" s="10">
         <v>222</v>
       </c>
       <c r="E10" t="s" s="7">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F10" s="10">
         <v>22</v>
@@ -1872,42 +1938,45 @@
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
       <c r="L10" t="s" s="7">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M10" s="12">
         <v>44216</v>
       </c>
       <c r="N10" t="s" s="7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O10" t="s" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P10" t="s" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q10" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R10" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="S10" t="s" s="7">
+        <v>28</v>
       </c>
     </row>
     <row r="11" ht="13.75" customHeight="1">
       <c r="A11" t="s" s="7">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B11" s="10">
         <v>2</v>
       </c>
       <c r="C11" t="s" s="7">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D11" s="10">
         <v>222</v>
       </c>
       <c r="E11" t="s" s="7">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F11" s="10">
         <v>33</v>
@@ -1922,25 +1991,28 @@
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
       <c r="L11" t="s" s="7">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M11" s="12">
         <v>44216</v>
       </c>
       <c r="N11" t="s" s="7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O11" t="s" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P11" t="s" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q11" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R11" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="S11" t="s" s="7">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore(condo): DOMA-7423 updated meter import example
</commit_message>
<xml_diff>
--- a/apps/condo/public/meter-import-example-en.xlsx
+++ b/apps/condo/public/meter-import-example-en.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
   <si>
     <t>Address</t>
   </si>
@@ -100,15 +100,27 @@
     <t>Kitchen</t>
   </si>
   <si>
+    <t>Parking place</t>
+  </si>
+  <si>
     <t>Bathroom</t>
   </si>
   <si>
+    <t>Apartment</t>
+  </si>
+  <si>
     <t>CW</t>
   </si>
   <si>
+    <t>Warehouse unit</t>
+  </si>
+  <si>
     <t>2021-12</t>
   </si>
   <si>
+    <t>Commercial unit</t>
+  </si>
+  <si>
     <t>EL</t>
   </si>
   <si>
@@ -116,9 +128,6 @@
   </si>
   <si>
     <t>г Москва, ул Тверская, д 2</t>
-  </si>
-  <si>
-    <t>Parking place</t>
   </si>
   <si>
     <t>2021-12-21</t>
@@ -151,9 +160,9 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="15"/>
       <color indexed="8"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="10"/>
@@ -552,7 +561,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -582,7 +590,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -608,7 +615,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -634,7 +640,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -660,7 +665,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -686,7 +690,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -712,7 +715,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -738,7 +740,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -764,7 +765,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -790,7 +790,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -841,7 +840,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -867,7 +865,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -893,7 +890,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -919,7 +915,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -945,7 +940,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -971,7 +965,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -997,7 +990,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1023,7 +1015,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1049,7 +1040,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1075,7 +1065,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1123,7 +1112,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1153,7 +1141,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1179,7 +1166,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1205,7 +1191,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1231,7 +1216,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1257,7 +1241,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1283,7 +1266,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1309,7 +1291,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1335,7 +1316,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1361,7 +1341,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1534,7 +1513,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s" s="7">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D3" s="10">
         <v>111</v>
@@ -1576,7 +1555,7 @@
         <v>27</v>
       </c>
       <c r="S3" t="s" s="7">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" ht="13.75" customHeight="1">
@@ -1587,13 +1566,13 @@
         <v>1</v>
       </c>
       <c r="C4" t="s" s="7">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D4" s="10">
         <v>111</v>
       </c>
       <c r="E4" t="s" s="7">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F4" s="10">
         <v>2</v>
@@ -1640,13 +1619,13 @@
         <v>1</v>
       </c>
       <c r="C5" t="s" s="7">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="D5" s="10">
         <v>111</v>
       </c>
       <c r="E5" t="s" s="7">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F5" s="10">
         <v>2</v>
@@ -1661,7 +1640,7 @@
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
       <c r="L5" t="s" s="7">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="M5" s="12">
         <v>44216</v>
@@ -1682,7 +1661,7 @@
         <v>27</v>
       </c>
       <c r="S5" t="s" s="7">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" ht="13.75" customHeight="1">
@@ -1693,13 +1672,13 @@
         <v>1</v>
       </c>
       <c r="C6" t="s" s="7">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="D6" s="10">
         <v>111</v>
       </c>
       <c r="E6" t="s" s="7">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F6" s="10">
         <v>2</v>
@@ -1718,7 +1697,7 @@
       </c>
       <c r="K6" s="11"/>
       <c r="L6" t="s" s="7">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="M6" s="12">
         <v>44216</v>
@@ -1756,7 +1735,7 @@
         <v>111</v>
       </c>
       <c r="E7" t="s" s="7">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F7" s="10">
         <v>2</v>
@@ -1796,24 +1775,24 @@
         <v>27</v>
       </c>
       <c r="S7" t="s" s="7">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" ht="13.75" customHeight="1">
       <c r="A8" t="s" s="7">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B8" s="10">
         <v>2</v>
       </c>
       <c r="C8" t="s" s="7">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D8" s="10">
         <v>222</v>
       </c>
       <c r="E8" t="s" s="7">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F8" s="10">
         <v>11</v>
@@ -1832,7 +1811,7 @@
       </c>
       <c r="K8" s="11"/>
       <c r="L8" t="s" s="7">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="M8" s="12">
         <v>44216</v>
@@ -1858,19 +1837,19 @@
     </row>
     <row r="9" ht="13.75" customHeight="1">
       <c r="A9" t="s" s="7">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B9" s="10">
         <v>2</v>
       </c>
       <c r="C9" t="s" s="7">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D9" s="10">
         <v>222</v>
       </c>
       <c r="E9" t="s" s="7">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F9" s="10">
         <v>11</v>
@@ -1885,7 +1864,7 @@
       <c r="J9" s="11"/>
       <c r="K9" s="11"/>
       <c r="L9" t="s" s="7">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="M9" s="12">
         <v>44216</v>
@@ -1906,24 +1885,24 @@
         <v>27</v>
       </c>
       <c r="S9" t="s" s="7">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" ht="13.75" customHeight="1">
       <c r="A10" t="s" s="7">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B10" s="10">
         <v>2</v>
       </c>
       <c r="C10" t="s" s="7">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D10" s="10">
         <v>222</v>
       </c>
       <c r="E10" t="s" s="7">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F10" s="10">
         <v>22</v>
@@ -1938,7 +1917,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
       <c r="L10" t="s" s="7">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="M10" s="12">
         <v>44216</v>
@@ -1964,19 +1943,19 @@
     </row>
     <row r="11" ht="13.75" customHeight="1">
       <c r="A11" t="s" s="7">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B11" s="10">
         <v>2</v>
       </c>
       <c r="C11" t="s" s="7">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D11" s="10">
         <v>222</v>
       </c>
       <c r="E11" t="s" s="7">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F11" s="10">
         <v>33</v>
@@ -1991,7 +1970,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
       <c r="L11" t="s" s="7">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="M11" s="12">
         <v>44216</v>
@@ -2012,7 +1991,7 @@
         <v>27</v>
       </c>
       <c r="S11" t="s" s="7">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore(condo): DOMA-7423 updated meter import example (#4022)
</commit_message>
<xml_diff>
--- a/apps/condo/public/meter-import-example-en.xlsx
+++ b/apps/condo/public/meter-import-example-en.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
   <si>
     <t>Address</t>
   </si>
@@ -100,15 +100,27 @@
     <t>Kitchen</t>
   </si>
   <si>
+    <t>Parking place</t>
+  </si>
+  <si>
     <t>Bathroom</t>
   </si>
   <si>
+    <t>Apartment</t>
+  </si>
+  <si>
     <t>CW</t>
   </si>
   <si>
+    <t>Warehouse unit</t>
+  </si>
+  <si>
     <t>2021-12</t>
   </si>
   <si>
+    <t>Commercial unit</t>
+  </si>
+  <si>
     <t>EL</t>
   </si>
   <si>
@@ -116,9 +128,6 @@
   </si>
   <si>
     <t>г Москва, ул Тверская, д 2</t>
-  </si>
-  <si>
-    <t>Parking place</t>
   </si>
   <si>
     <t>2021-12-21</t>
@@ -151,9 +160,9 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="15"/>
       <color indexed="8"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="10"/>
@@ -552,7 +561,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -582,7 +590,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -608,7 +615,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -634,7 +640,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -660,7 +665,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -686,7 +690,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -712,7 +715,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -738,7 +740,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -764,7 +765,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -790,7 +790,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -841,7 +840,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -867,7 +865,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -893,7 +890,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -919,7 +915,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -945,7 +940,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -971,7 +965,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -997,7 +990,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1023,7 +1015,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1049,7 +1040,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1075,7 +1065,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1123,7 +1112,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1153,7 +1141,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1179,7 +1166,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1205,7 +1191,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1231,7 +1216,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1257,7 +1241,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1283,7 +1266,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1309,7 +1291,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1335,7 +1316,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1361,7 +1341,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1534,7 +1513,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s" s="7">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D3" s="10">
         <v>111</v>
@@ -1576,7 +1555,7 @@
         <v>27</v>
       </c>
       <c r="S3" t="s" s="7">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" ht="13.75" customHeight="1">
@@ -1587,13 +1566,13 @@
         <v>1</v>
       </c>
       <c r="C4" t="s" s="7">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D4" s="10">
         <v>111</v>
       </c>
       <c r="E4" t="s" s="7">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F4" s="10">
         <v>2</v>
@@ -1640,13 +1619,13 @@
         <v>1</v>
       </c>
       <c r="C5" t="s" s="7">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="D5" s="10">
         <v>111</v>
       </c>
       <c r="E5" t="s" s="7">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F5" s="10">
         <v>2</v>
@@ -1661,7 +1640,7 @@
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
       <c r="L5" t="s" s="7">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="M5" s="12">
         <v>44216</v>
@@ -1682,7 +1661,7 @@
         <v>27</v>
       </c>
       <c r="S5" t="s" s="7">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" ht="13.75" customHeight="1">
@@ -1693,13 +1672,13 @@
         <v>1</v>
       </c>
       <c r="C6" t="s" s="7">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="D6" s="10">
         <v>111</v>
       </c>
       <c r="E6" t="s" s="7">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F6" s="10">
         <v>2</v>
@@ -1718,7 +1697,7 @@
       </c>
       <c r="K6" s="11"/>
       <c r="L6" t="s" s="7">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="M6" s="12">
         <v>44216</v>
@@ -1756,7 +1735,7 @@
         <v>111</v>
       </c>
       <c r="E7" t="s" s="7">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F7" s="10">
         <v>2</v>
@@ -1796,24 +1775,24 @@
         <v>27</v>
       </c>
       <c r="S7" t="s" s="7">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" ht="13.75" customHeight="1">
       <c r="A8" t="s" s="7">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B8" s="10">
         <v>2</v>
       </c>
       <c r="C8" t="s" s="7">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D8" s="10">
         <v>222</v>
       </c>
       <c r="E8" t="s" s="7">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F8" s="10">
         <v>11</v>
@@ -1832,7 +1811,7 @@
       </c>
       <c r="K8" s="11"/>
       <c r="L8" t="s" s="7">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="M8" s="12">
         <v>44216</v>
@@ -1858,19 +1837,19 @@
     </row>
     <row r="9" ht="13.75" customHeight="1">
       <c r="A9" t="s" s="7">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B9" s="10">
         <v>2</v>
       </c>
       <c r="C9" t="s" s="7">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D9" s="10">
         <v>222</v>
       </c>
       <c r="E9" t="s" s="7">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F9" s="10">
         <v>11</v>
@@ -1885,7 +1864,7 @@
       <c r="J9" s="11"/>
       <c r="K9" s="11"/>
       <c r="L9" t="s" s="7">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="M9" s="12">
         <v>44216</v>
@@ -1906,24 +1885,24 @@
         <v>27</v>
       </c>
       <c r="S9" t="s" s="7">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" ht="13.75" customHeight="1">
       <c r="A10" t="s" s="7">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B10" s="10">
         <v>2</v>
       </c>
       <c r="C10" t="s" s="7">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D10" s="10">
         <v>222</v>
       </c>
       <c r="E10" t="s" s="7">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F10" s="10">
         <v>22</v>
@@ -1938,7 +1917,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
       <c r="L10" t="s" s="7">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="M10" s="12">
         <v>44216</v>
@@ -1964,19 +1943,19 @@
     </row>
     <row r="11" ht="13.75" customHeight="1">
       <c r="A11" t="s" s="7">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B11" s="10">
         <v>2</v>
       </c>
       <c r="C11" t="s" s="7">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D11" s="10">
         <v>222</v>
       </c>
       <c r="E11" t="s" s="7">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F11" s="10">
         <v>33</v>
@@ -1991,7 +1970,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
       <c r="L11" t="s" s="7">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="M11" s="12">
         <v>44216</v>
@@ -2012,7 +1991,7 @@
         <v>27</v>
       </c>
       <c r="S11" t="s" s="7">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>